<commit_message>
Fix positive model output to match diagnostics script
</commit_message>
<xml_diff>
--- a/goaTrawl/_Species Models.xlsx
+++ b/goaTrawl/_Species Models.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14080" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="800" yWindow="240" windowWidth="17920" windowHeight="14680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="94">
   <si>
     <t>Species</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>Atheresthes.stomias</t>
+  </si>
+  <si>
+    <t>running</t>
   </si>
 </sst>
 </file>
@@ -407,8 +410,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="213">
+  <cellStyleXfs count="215">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -649,7 +654,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="213">
+  <cellStyles count="215">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -756,6 +761,7 @@
     <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -862,6 +868,7 @@
     <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1193,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="L26" workbookViewId="0">
+      <selection activeCell="S37" sqref="S37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1279,10 +1286,10 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="17" t="s">
@@ -1292,7 +1299,7 @@
         <v>11</v>
       </c>
       <c r="F3">
-        <v>718</v>
+        <v>9444</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -1301,15 +1308,17 @@
         <v>92</v>
       </c>
       <c r="N3" s="5"/>
-      <c r="O3" s="7"/>
+      <c r="O3" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P3" s="7"/>
     </row>
     <row r="4" spans="1:19">
       <c r="A4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="17" t="s">
@@ -1319,7 +1328,7 @@
         <v>11</v>
       </c>
       <c r="F4">
-        <v>4666</v>
+        <v>8006</v>
       </c>
       <c r="L4">
         <v>2</v>
@@ -1328,15 +1337,17 @@
         <v>39</v>
       </c>
       <c r="N4" s="5"/>
-      <c r="O4" s="8"/>
+      <c r="O4" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="P4" s="8"/>
     </row>
     <row r="5" spans="1:19">
       <c r="A5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="17" t="s">
@@ -1346,7 +1357,7 @@
         <v>11</v>
       </c>
       <c r="F5">
-        <v>9444</v>
+        <v>7458</v>
       </c>
       <c r="L5">
         <v>3</v>
@@ -1355,15 +1366,17 @@
         <v>40</v>
       </c>
       <c r="N5" s="5"/>
-      <c r="O5" s="8"/>
+      <c r="O5" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="P5" s="8"/>
     </row>
     <row r="6" spans="1:19">
       <c r="A6">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="17" t="s">
@@ -1373,7 +1386,7 @@
         <v>11</v>
       </c>
       <c r="F6">
-        <v>1363</v>
+        <v>6913</v>
       </c>
       <c r="L6">
         <v>4</v>
@@ -1382,15 +1395,17 @@
         <v>41</v>
       </c>
       <c r="N6" s="5"/>
-      <c r="O6" s="7"/>
+      <c r="O6" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P6" s="7"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="17" t="s">
@@ -1400,7 +1415,7 @@
         <v>11</v>
       </c>
       <c r="F7">
-        <v>823</v>
+        <v>6809</v>
       </c>
       <c r="L7">
         <v>5</v>
@@ -1409,15 +1424,17 @@
         <v>42</v>
       </c>
       <c r="N7" s="5"/>
-      <c r="O7" s="7"/>
+      <c r="O7" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P7" s="7"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="17" t="s">
@@ -1427,7 +1444,7 @@
         <v>11</v>
       </c>
       <c r="F8">
-        <v>885</v>
+        <v>5668</v>
       </c>
       <c r="L8">
         <v>6</v>
@@ -1436,15 +1453,17 @@
         <v>43</v>
       </c>
       <c r="N8" s="5"/>
-      <c r="O8" s="7"/>
+      <c r="O8" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P8" s="7"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="17" t="s">
@@ -1454,7 +1473,7 @@
         <v>11</v>
       </c>
       <c r="F9">
-        <v>2013</v>
+        <v>5337</v>
       </c>
       <c r="L9">
         <v>7</v>
@@ -1463,15 +1482,17 @@
         <v>44</v>
       </c>
       <c r="N9" s="5"/>
-      <c r="O9" s="8"/>
+      <c r="O9" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="P9" s="8"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="17" t="s">
@@ -1481,7 +1502,7 @@
         <v>11</v>
       </c>
       <c r="F10">
-        <v>709</v>
+        <v>4666</v>
       </c>
       <c r="L10">
         <v>8</v>
@@ -1490,15 +1511,17 @@
         <v>45</v>
       </c>
       <c r="N10" s="5"/>
-      <c r="O10" s="8"/>
+      <c r="O10" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="P10" s="8"/>
     </row>
     <row r="11" spans="1:19">
       <c r="A11">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="17" t="s">
@@ -1508,7 +1531,7 @@
         <v>11</v>
       </c>
       <c r="F11">
-        <v>1221</v>
+        <v>4344</v>
       </c>
       <c r="L11">
         <v>9</v>
@@ -1517,15 +1540,17 @@
         <v>46</v>
       </c>
       <c r="N11" s="5"/>
-      <c r="O11" s="7"/>
+      <c r="O11" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P11" s="7"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="17" t="s">
@@ -1534,6 +1559,9 @@
       <c r="E12" s="17" t="s">
         <v>11</v>
       </c>
+      <c r="F12">
+        <v>3163</v>
+      </c>
       <c r="L12">
         <v>10</v>
       </c>
@@ -1541,15 +1569,17 @@
         <v>47</v>
       </c>
       <c r="N12" s="5"/>
-      <c r="O12" s="7"/>
+      <c r="O12" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P12" s="7"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="17" t="s">
@@ -1559,7 +1589,7 @@
         <v>11</v>
       </c>
       <c r="F13">
-        <v>7458</v>
+        <v>2662</v>
       </c>
       <c r="L13">
         <v>11</v>
@@ -1568,15 +1598,17 @@
         <v>48</v>
       </c>
       <c r="N13" s="5"/>
-      <c r="O13" s="7"/>
+      <c r="O13" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P13" s="7"/>
     </row>
     <row r="14" spans="1:19">
       <c r="A14">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="17" t="s">
@@ -1586,7 +1618,7 @@
         <v>11</v>
       </c>
       <c r="F14">
-        <v>6913</v>
+        <v>2411</v>
       </c>
       <c r="L14">
         <v>12</v>
@@ -1595,15 +1627,17 @@
         <v>49</v>
       </c>
       <c r="N14" s="5"/>
-      <c r="O14" s="8"/>
+      <c r="O14" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="P14" s="8"/>
     </row>
     <row r="15" spans="1:19">
       <c r="A15">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="17" t="s">
@@ -1613,7 +1647,7 @@
         <v>11</v>
       </c>
       <c r="F15">
-        <v>6809</v>
+        <v>2013</v>
       </c>
       <c r="L15">
         <v>13</v>
@@ -1622,15 +1656,17 @@
         <v>50</v>
       </c>
       <c r="N15" s="5"/>
-      <c r="O15" s="8"/>
+      <c r="O15" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="P15" s="8"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="17" t="s">
@@ -1640,7 +1676,7 @@
         <v>11</v>
       </c>
       <c r="F16">
-        <v>2411</v>
+        <v>1876</v>
       </c>
       <c r="L16">
         <v>14</v>
@@ -1649,15 +1685,17 @@
         <v>51</v>
       </c>
       <c r="N16" s="5"/>
-      <c r="O16" s="8"/>
+      <c r="O16" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="P16" s="8"/>
     </row>
     <row r="17" spans="1:16">
       <c r="A17">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="17" t="s">
@@ -1667,7 +1705,7 @@
         <v>11</v>
       </c>
       <c r="F17">
-        <v>1185</v>
+        <v>1812</v>
       </c>
       <c r="L17">
         <v>15</v>
@@ -1676,15 +1714,17 @@
         <v>52</v>
       </c>
       <c r="N17" s="5"/>
-      <c r="O17" s="7"/>
+      <c r="O17" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P17" s="7"/>
     </row>
     <row r="18" spans="1:16">
       <c r="A18">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="17" t="s">
@@ -1694,7 +1734,7 @@
         <v>11</v>
       </c>
       <c r="F18">
-        <v>661</v>
+        <v>1802</v>
       </c>
       <c r="L18">
         <v>16</v>
@@ -1703,15 +1743,17 @@
         <v>53</v>
       </c>
       <c r="N18" s="5"/>
-      <c r="O18" s="7"/>
+      <c r="O18" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P18" s="7"/>
     </row>
     <row r="19" spans="1:16">
       <c r="A19">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="17" t="s">
@@ -1720,9 +1762,6 @@
       <c r="E19" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F19">
-        <v>5668</v>
-      </c>
       <c r="L19">
         <v>17</v>
       </c>
@@ -1730,15 +1769,17 @@
         <v>54</v>
       </c>
       <c r="N19" s="5"/>
-      <c r="O19" s="8"/>
+      <c r="O19" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="P19" s="8"/>
     </row>
     <row r="20" spans="1:16">
       <c r="A20">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="17" t="s">
@@ -1748,7 +1789,7 @@
         <v>11</v>
       </c>
       <c r="F20">
-        <v>8006</v>
+        <v>1363</v>
       </c>
       <c r="L20">
         <v>18</v>
@@ -1757,15 +1798,17 @@
         <v>55</v>
       </c>
       <c r="N20" s="5"/>
-      <c r="O20" s="8"/>
+      <c r="O20" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="P20" s="8"/>
     </row>
     <row r="21" spans="1:16">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="17" t="s">
@@ -1775,7 +1818,7 @@
         <v>11</v>
       </c>
       <c r="F21">
-        <v>1289</v>
+        <v>1296</v>
       </c>
       <c r="L21">
         <v>19</v>
@@ -1784,15 +1827,17 @@
         <v>56</v>
       </c>
       <c r="N21" s="5"/>
-      <c r="O21" s="7"/>
+      <c r="O21" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P21" s="7"/>
     </row>
     <row r="22" spans="1:16">
       <c r="A22">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="17" t="s">
@@ -1802,7 +1847,7 @@
         <v>11</v>
       </c>
       <c r="F22">
-        <v>641</v>
+        <v>1289</v>
       </c>
       <c r="L22">
         <v>20</v>
@@ -1811,15 +1856,17 @@
         <v>57</v>
       </c>
       <c r="N22" s="5"/>
-      <c r="O22" s="7"/>
+      <c r="O22" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P22" s="7"/>
     </row>
     <row r="23" spans="1:16">
       <c r="A23">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="17" t="s">
@@ -1829,7 +1876,7 @@
         <v>11</v>
       </c>
       <c r="F23">
-        <v>960</v>
+        <v>1225</v>
       </c>
       <c r="L23">
         <v>21</v>
@@ -1837,16 +1884,18 @@
       <c r="M23" t="s">
         <v>58</v>
       </c>
-      <c r="N23" s="5"/>
+      <c r="N23" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
     </row>
     <row r="24" spans="1:16">
       <c r="A24">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="17" t="s">
@@ -1855,22 +1904,27 @@
       <c r="E24" s="17" t="s">
         <v>11</v>
       </c>
+      <c r="F24">
+        <v>1221</v>
+      </c>
       <c r="L24">
         <v>22</v>
       </c>
       <c r="M24" t="s">
         <v>59</v>
       </c>
-      <c r="N24" s="5"/>
+      <c r="N24" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="O24" s="8"/>
       <c r="P24" s="8"/>
     </row>
     <row r="25" spans="1:16">
       <c r="A25">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="17" t="s">
@@ -1880,7 +1934,7 @@
         <v>11</v>
       </c>
       <c r="F25">
-        <v>649</v>
+        <v>1185</v>
       </c>
       <c r="L25">
         <v>23</v>
@@ -1888,7 +1942,9 @@
       <c r="M25" t="s">
         <v>60</v>
       </c>
-      <c r="N25" s="5"/>
+      <c r="N25" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
     </row>
@@ -1915,16 +1971,18 @@
       <c r="M26" t="s">
         <v>61</v>
       </c>
-      <c r="N26" s="5"/>
+      <c r="N26" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="O26" s="7"/>
       <c r="P26" s="7"/>
     </row>
     <row r="27" spans="1:16">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="17" t="s">
@@ -1934,7 +1992,7 @@
         <v>11</v>
       </c>
       <c r="F27">
-        <v>1103</v>
+        <v>1115</v>
       </c>
       <c r="L27">
         <v>25</v>
@@ -1942,16 +2000,18 @@
       <c r="M27" t="s">
         <v>62</v>
       </c>
-      <c r="N27" s="5"/>
+      <c r="N27" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="O27" s="7"/>
       <c r="P27" s="7"/>
     </row>
     <row r="28" spans="1:16">
       <c r="A28">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="17" t="s">
@@ -1961,7 +2021,7 @@
         <v>11</v>
       </c>
       <c r="F28">
-        <v>707</v>
+        <v>1103</v>
       </c>
       <c r="L28">
         <v>26</v>
@@ -1970,15 +2030,17 @@
         <v>63</v>
       </c>
       <c r="N28" s="5"/>
-      <c r="O28" s="7"/>
+      <c r="O28" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P28" s="7"/>
     </row>
     <row r="29" spans="1:16">
       <c r="A29">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="17" t="s">
@@ -1988,7 +2050,7 @@
         <v>11</v>
       </c>
       <c r="F29">
-        <v>1225</v>
+        <v>1083</v>
       </c>
       <c r="L29">
         <v>27</v>
@@ -1997,15 +2059,17 @@
         <v>64</v>
       </c>
       <c r="N29" s="5"/>
-      <c r="O29" s="7"/>
+      <c r="O29" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P29" s="7"/>
     </row>
     <row r="30" spans="1:16">
       <c r="A30">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="17" t="s">
@@ -2015,7 +2079,7 @@
         <v>11</v>
       </c>
       <c r="F30">
-        <v>1296</v>
+        <v>998</v>
       </c>
       <c r="L30">
         <v>28</v>
@@ -2024,23 +2088,27 @@
         <v>65</v>
       </c>
       <c r="N30" s="5"/>
-      <c r="O30" s="7"/>
+      <c r="O30" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P30" s="7"/>
     </row>
     <row r="31" spans="1:16">
       <c r="A31">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="17"/>
+      <c r="E31" s="17" t="s">
+        <v>11</v>
+      </c>
       <c r="F31">
-        <v>323</v>
+        <v>960</v>
       </c>
       <c r="L31">
         <v>29</v>
@@ -2049,15 +2117,17 @@
         <v>66</v>
       </c>
       <c r="N31" s="5"/>
-      <c r="O31" s="7"/>
+      <c r="O31" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P31" s="7"/>
     </row>
     <row r="32" spans="1:16">
       <c r="A32">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="17" t="s">
@@ -2067,7 +2137,7 @@
         <v>11</v>
       </c>
       <c r="F32">
-        <v>5337</v>
+        <v>927</v>
       </c>
       <c r="L32">
         <v>30</v>
@@ -2076,15 +2146,17 @@
         <v>67</v>
       </c>
       <c r="N32" s="5"/>
-      <c r="O32" s="8"/>
+      <c r="O32" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="P32" s="8"/>
     </row>
     <row r="33" spans="1:16">
       <c r="A33">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="17" t="s">
@@ -2094,7 +2166,7 @@
         <v>11</v>
       </c>
       <c r="F33">
-        <v>313</v>
+        <v>885</v>
       </c>
       <c r="L33">
         <v>31</v>
@@ -2135,10 +2207,10 @@
     </row>
     <row r="35" spans="1:16">
       <c r="A35">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="17" t="s">
@@ -2148,7 +2220,7 @@
         <v>11</v>
       </c>
       <c r="F35">
-        <v>683</v>
+        <v>873</v>
       </c>
       <c r="L35">
         <v>33</v>
@@ -2162,12 +2234,12 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>86</v>
-      </c>
-      <c r="C36" s="5"/>
+        <v>71</v>
+      </c>
+      <c r="C36" s="6"/>
       <c r="D36" s="17" t="s">
         <v>11</v>
       </c>
@@ -2175,7 +2247,7 @@
         <v>11</v>
       </c>
       <c r="F36">
-        <v>581</v>
+        <v>825</v>
       </c>
       <c r="L36">
         <v>34</v>
@@ -2189,10 +2261,10 @@
     </row>
     <row r="37" spans="1:16">
       <c r="A37">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="17" t="s">
@@ -2202,7 +2274,7 @@
         <v>11</v>
       </c>
       <c r="F37">
-        <v>1083</v>
+        <v>824</v>
       </c>
       <c r="L37">
         <v>35</v>
@@ -2216,12 +2288,12 @@
     </row>
     <row r="38" spans="1:16">
       <c r="A38">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
-      </c>
-      <c r="C38" s="6"/>
+        <v>73</v>
+      </c>
+      <c r="C38" s="5"/>
       <c r="D38" s="17" t="s">
         <v>11</v>
       </c>
@@ -2229,7 +2301,7 @@
         <v>11</v>
       </c>
       <c r="F38">
-        <v>787</v>
+        <v>823</v>
       </c>
       <c r="L38">
         <v>36</v>
@@ -2243,12 +2315,12 @@
     </row>
     <row r="39" spans="1:16">
       <c r="A39">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="5"/>
+        <v>74</v>
+      </c>
+      <c r="C39" s="6"/>
       <c r="D39" s="17" t="s">
         <v>11</v>
       </c>
@@ -2256,7 +2328,7 @@
         <v>11</v>
       </c>
       <c r="F39">
-        <v>667</v>
+        <v>787</v>
       </c>
       <c r="L39">
         <v>37</v>
@@ -2270,10 +2342,10 @@
     </row>
     <row r="40" spans="1:16">
       <c r="A40">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="17" t="s">
@@ -2283,7 +2355,7 @@
         <v>11</v>
       </c>
       <c r="F40">
-        <v>927</v>
+        <v>751</v>
       </c>
       <c r="L40">
         <v>38</v>
@@ -2297,10 +2369,10 @@
     </row>
     <row r="41" spans="1:16">
       <c r="A41">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="17" t="s">
@@ -2310,7 +2382,7 @@
         <v>11</v>
       </c>
       <c r="F41">
-        <v>495</v>
+        <v>718</v>
       </c>
       <c r="L41">
         <v>39</v>
@@ -2324,20 +2396,18 @@
     </row>
     <row r="42" spans="1:16">
       <c r="A42">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C42" s="5"/>
-      <c r="D42" s="17" t="s">
-        <v>11</v>
-      </c>
+      <c r="D42" s="17"/>
       <c r="E42" s="17" t="s">
         <v>11</v>
       </c>
       <c r="F42">
-        <v>627</v>
+        <v>718</v>
       </c>
       <c r="L42">
         <v>40</v>
@@ -2351,10 +2421,10 @@
     </row>
     <row r="43" spans="1:16">
       <c r="A43">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="17" t="s">
@@ -2364,7 +2434,7 @@
         <v>11</v>
       </c>
       <c r="F43">
-        <v>998</v>
+        <v>709</v>
       </c>
       <c r="L43">
         <v>41</v>
@@ -2378,10 +2448,10 @@
     </row>
     <row r="44" spans="1:16">
       <c r="A44">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="17" t="s">
@@ -2391,7 +2461,7 @@
         <v>11</v>
       </c>
       <c r="F44">
-        <v>1876</v>
+        <v>707</v>
       </c>
       <c r="L44">
         <v>42</v>
@@ -2405,10 +2475,10 @@
     </row>
     <row r="45" spans="1:16">
       <c r="A45">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="17" t="s">
@@ -2416,6 +2486,9 @@
       </c>
       <c r="E45" s="17" t="s">
         <v>11</v>
+      </c>
+      <c r="F45">
+        <v>683</v>
       </c>
       <c r="L45">
         <v>43</v>
@@ -2429,10 +2502,10 @@
     </row>
     <row r="46" spans="1:16">
       <c r="A46">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="17" t="s">
@@ -2442,7 +2515,7 @@
         <v>11</v>
       </c>
       <c r="F46">
-        <v>4344</v>
+        <v>667</v>
       </c>
       <c r="L46">
         <v>44</v>
@@ -2456,10 +2529,10 @@
     </row>
     <row r="47" spans="1:16">
       <c r="A47">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="17" t="s">
@@ -2469,7 +2542,7 @@
         <v>11</v>
       </c>
       <c r="F47">
-        <v>1115</v>
+        <v>661</v>
       </c>
       <c r="L47">
         <v>45</v>
@@ -2483,10 +2556,10 @@
     </row>
     <row r="48" spans="1:16">
       <c r="A48">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="17" t="s">
@@ -2496,7 +2569,7 @@
         <v>11</v>
       </c>
       <c r="F48">
-        <v>873</v>
+        <v>649</v>
       </c>
       <c r="L48">
         <v>46</v>
@@ -2510,18 +2583,20 @@
     </row>
     <row r="49" spans="1:20">
       <c r="A49">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C49" s="5"/>
-      <c r="D49" s="17"/>
+      <c r="D49" s="17" t="s">
+        <v>11</v>
+      </c>
       <c r="E49" s="17" t="s">
         <v>11</v>
       </c>
       <c r="F49">
-        <v>718</v>
+        <v>641</v>
       </c>
       <c r="L49">
         <v>47</v>
@@ -2535,10 +2610,10 @@
     </row>
     <row r="50" spans="1:20">
       <c r="A50">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="17" t="s">
@@ -2548,7 +2623,7 @@
         <v>11</v>
       </c>
       <c r="F50">
-        <v>1812</v>
+        <v>627</v>
       </c>
       <c r="L50">
         <v>48</v>
@@ -2562,10 +2637,10 @@
     </row>
     <row r="51" spans="1:20">
       <c r="A51">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="17" t="s">
@@ -2575,7 +2650,7 @@
         <v>11</v>
       </c>
       <c r="F51">
-        <v>307</v>
+        <v>581</v>
       </c>
       <c r="L51">
         <v>49</v>
@@ -2589,10 +2664,10 @@
     </row>
     <row r="52" spans="1:20">
       <c r="A52">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="17" t="s">
@@ -2602,7 +2677,7 @@
         <v>11</v>
       </c>
       <c r="F52">
-        <v>824</v>
+        <v>495</v>
       </c>
       <c r="L52">
         <v>50</v>
@@ -2616,20 +2691,18 @@
     </row>
     <row r="53" spans="1:20">
       <c r="A53">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>71</v>
-      </c>
-      <c r="C53" s="6"/>
+        <v>88</v>
+      </c>
+      <c r="C53" s="5"/>
       <c r="D53" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E53" s="17" t="s">
-        <v>11</v>
-      </c>
+      <c r="E53" s="17"/>
       <c r="F53">
-        <v>825</v>
+        <v>323</v>
       </c>
       <c r="L53">
         <v>51</v>
@@ -2643,10 +2716,10 @@
     </row>
     <row r="54" spans="1:20">
       <c r="A54">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="17" t="s">
@@ -2656,7 +2729,7 @@
         <v>11</v>
       </c>
       <c r="F54">
-        <v>2662</v>
+        <v>313</v>
       </c>
       <c r="L54">
         <v>52</v>
@@ -2670,10 +2743,10 @@
     </row>
     <row r="55" spans="1:20">
       <c r="A55">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="17" t="s">
@@ -2683,7 +2756,7 @@
         <v>11</v>
       </c>
       <c r="F55">
-        <v>1802</v>
+        <v>307</v>
       </c>
       <c r="L55">
         <v>53</v>
@@ -2697,10 +2770,10 @@
     </row>
     <row r="56" spans="1:20">
       <c r="A56">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="17" t="s">
@@ -2708,9 +2781,6 @@
       </c>
       <c r="E56" s="17" t="s">
         <v>11</v>
-      </c>
-      <c r="F56">
-        <v>3163</v>
       </c>
       <c r="L56">
         <v>54</v>
@@ -2724,10 +2794,10 @@
     </row>
     <row r="57" spans="1:20">
       <c r="A57">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="17" t="s">
@@ -2735,9 +2805,6 @@
       </c>
       <c r="E57" s="17" t="s">
         <v>11</v>
-      </c>
-      <c r="F57">
-        <v>751</v>
       </c>
       <c r="L57">
         <v>55</v>
@@ -3394,7 +3461,7 @@
     </row>
   </sheetData>
   <sortState ref="A3:F57">
-    <sortCondition ref="B3:B57"/>
+    <sortCondition ref="A3:A57"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="D1:E1"/>

</xml_diff>

<commit_message>
Resolve projecting code for index standardization and for spatial map making.
</commit_message>
<xml_diff>
--- a/goaTrawl/_Species Models.xlsx
+++ b/goaTrawl/_Species Models.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="240" windowWidth="17920" windowHeight="14680" tabRatio="500"/>
+    <workbookView xWindow="1920" yWindow="0" windowWidth="17920" windowHeight="14680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="96">
   <si>
     <t>Species</t>
   </si>
@@ -301,6 +301,12 @@
   </si>
   <si>
     <t>running</t>
+  </si>
+  <si>
+    <t>DIC +2</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -410,7 +416,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="215">
+  <cellStyleXfs count="289">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -626,8 +632,82 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -653,8 +733,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="215">
+  <cellStyles count="289">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -762,6 +843,43 @@
     <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -869,6 +987,43 @@
     <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1200,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L26" workbookViewId="0">
-      <selection activeCell="S37" sqref="S37"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1301,17 +1456,23 @@
       <c r="F3">
         <v>9444</v>
       </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
       <c r="L3">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="M3" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="7" t="s">
         <v>11</v>
       </c>
       <c r="P3" s="7"/>
+      <c r="Q3">
+        <v>718</v>
+      </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4">
@@ -1330,17 +1491,28 @@
       <c r="F4">
         <v>8006</v>
       </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
       <c r="L4">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="8"/>
+      <c r="P4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4">
+        <v>4666</v>
+      </c>
+      <c r="R4" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5">
@@ -1359,17 +1531,28 @@
       <c r="F5">
         <v>7458</v>
       </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
       <c r="L5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="N5" s="5"/>
-      <c r="O5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P5" s="8"/>
+      <c r="O5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q5">
+        <v>9444</v>
+      </c>
+      <c r="R5" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6">
@@ -1388,17 +1571,28 @@
       <c r="F6">
         <v>6913</v>
       </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
       <c r="L6">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="M6" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="N6" s="5"/>
-      <c r="O6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="P6" s="7"/>
+      <c r="O6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q6">
+        <v>1363</v>
+      </c>
+      <c r="R6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7">
@@ -1417,17 +1611,23 @@
       <c r="F7">
         <v>6809</v>
       </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
       <c r="L7">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="M7" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="7" t="s">
         <v>11</v>
       </c>
       <c r="P7" s="7"/>
+      <c r="Q7">
+        <v>823</v>
+      </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8">
@@ -1446,17 +1646,28 @@
       <c r="F8">
         <v>5668</v>
       </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
       <c r="L8">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="M8" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="N8" s="5"/>
       <c r="O8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="7"/>
+      <c r="P8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q8">
+        <v>885</v>
+      </c>
+      <c r="R8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9">
@@ -1475,17 +1686,28 @@
       <c r="F9">
         <v>5337</v>
       </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
       <c r="L9">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="M9" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="N9" s="5"/>
       <c r="O9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="8"/>
+      <c r="P9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9">
+        <v>2013</v>
+      </c>
+      <c r="R9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:19">
       <c r="A10">
@@ -1504,17 +1726,23 @@
       <c r="F10">
         <v>4666</v>
       </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
       <c r="L10">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="M10" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="N10" s="5"/>
-      <c r="O10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P10" s="8"/>
+      <c r="O10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P10" s="7"/>
+      <c r="Q10">
+        <v>709</v>
+      </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11">
@@ -1533,17 +1761,28 @@
       <c r="F11">
         <v>4344</v>
       </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
       <c r="L11">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="M11" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="P11" s="7"/>
+      <c r="P11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q11">
+        <v>1221</v>
+      </c>
+      <c r="R11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12">
@@ -1562,17 +1801,23 @@
       <c r="F12">
         <v>3163</v>
       </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
       <c r="L12">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="M12" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="N12" s="5"/>
-      <c r="O12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="P12" s="7"/>
+      <c r="O12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="P12" s="8"/>
+      <c r="Q12">
+        <v>1763</v>
+      </c>
     </row>
     <row r="13" spans="1:19">
       <c r="A13">
@@ -1591,17 +1836,28 @@
       <c r="F13">
         <v>2662</v>
       </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
       <c r="L13">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="M13" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="N13" s="5"/>
-      <c r="O13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="P13" s="7"/>
+      <c r="O13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="P13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q13">
+        <v>7458</v>
+      </c>
+      <c r="R13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:19">
       <c r="A14">
@@ -1620,17 +1876,28 @@
       <c r="F14">
         <v>2411</v>
       </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
       <c r="L14">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="M14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="N14" s="5"/>
-      <c r="O14" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P14" s="8"/>
+      <c r="O14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q14">
+        <v>6913</v>
+      </c>
+      <c r="R14" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:19">
       <c r="A15">
@@ -1649,17 +1916,28 @@
       <c r="F15">
         <v>2013</v>
       </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
       <c r="L15">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="M15" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="N15" s="5"/>
-      <c r="O15" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P15" s="8"/>
+      <c r="O15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P15" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q15">
+        <v>6809</v>
+      </c>
+      <c r="R15" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:19">
       <c r="A16">
@@ -1678,19 +1956,30 @@
       <c r="F16">
         <v>1876</v>
       </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
       <c r="L16">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="N16" s="5"/>
       <c r="O16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P16" s="8"/>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="P16" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q16">
+        <v>2411</v>
+      </c>
+      <c r="R16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1707,19 +1996,32 @@
       <c r="F17">
         <v>1812</v>
       </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
       <c r="L17">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="M17" t="s">
-        <v>52</v>
-      </c>
-      <c r="N17" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="O17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="P17" s="7"/>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="P17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q17">
+        <v>1185</v>
+      </c>
+      <c r="R17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1736,19 +2038,25 @@
       <c r="F18">
         <v>1802</v>
       </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
       <c r="L18">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="M18" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="N18" s="5"/>
       <c r="O18" s="7" t="s">
         <v>11</v>
       </c>
       <c r="P18" s="7"/>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="Q18">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1762,19 +2070,33 @@
       <c r="E19" s="17" t="s">
         <v>11</v>
       </c>
+      <c r="F19">
+        <v>4617</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
       <c r="L19">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="M19" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="N19" s="5"/>
-      <c r="O19" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="P19" s="8"/>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="O19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q19">
+        <v>5668</v>
+      </c>
+      <c r="R19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1791,19 +2113,33 @@
       <c r="F20">
         <v>1363</v>
       </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>94</v>
+      </c>
       <c r="L20">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="M20" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="N20" s="5"/>
       <c r="O20" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P20" s="8"/>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="P20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q20">
+        <v>8006</v>
+      </c>
+      <c r="R20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1820,19 +2156,30 @@
       <c r="F21">
         <v>1296</v>
       </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
       <c r="L21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N21" s="5"/>
       <c r="O21" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="P21" s="7"/>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="P21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q21">
+        <v>1289</v>
+      </c>
+      <c r="R21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1849,19 +2196,25 @@
       <c r="F22">
         <v>1289</v>
       </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
       <c r="L22">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="M22" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="N22" s="5"/>
       <c r="O22" s="7" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="P22" s="7"/>
-    </row>
-    <row r="23" spans="1:16">
+      <c r="Q22">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1878,19 +2231,25 @@
       <c r="F23">
         <v>1225</v>
       </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
       <c r="L23">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="M23" t="s">
-        <v>58</v>
-      </c>
-      <c r="N23" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="O23" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="N23" s="5"/>
+      <c r="O23" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="P23" s="7"/>
-    </row>
-    <row r="24" spans="1:16">
+      <c r="Q23">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1907,19 +2266,30 @@
       <c r="F24">
         <v>1221</v>
       </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
       <c r="L24">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="M24" t="s">
-        <v>59</v>
-      </c>
-      <c r="N24" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-    </row>
-    <row r="25" spans="1:16">
+        <v>54</v>
+      </c>
+      <c r="N24" s="5"/>
+      <c r="O24" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="P24" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q24">
+        <v>4617</v>
+      </c>
+      <c r="R24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1936,19 +2306,25 @@
       <c r="F25">
         <v>1185</v>
       </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
       <c r="L25">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="M25" t="s">
-        <v>60</v>
-      </c>
-      <c r="N25" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="O25" s="7"/>
+        <v>83</v>
+      </c>
+      <c r="N25" s="5"/>
+      <c r="O25" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P25" s="7"/>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="Q25">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1965,6 +2341,9 @@
       <c r="F26">
         <v>1117</v>
       </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
       <c r="L26">
         <v>24</v>
       </c>
@@ -1974,10 +2353,20 @@
       <c r="N26" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="O26" s="7"/>
-      <c r="P26" s="7"/>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="O26" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P26" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q26">
+        <v>1117</v>
+      </c>
+      <c r="R26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1994,19 +2383,25 @@
       <c r="F27">
         <v>1115</v>
       </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
       <c r="L27">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M27" t="s">
-        <v>62</v>
-      </c>
-      <c r="N27" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="O27" s="7"/>
+        <v>63</v>
+      </c>
+      <c r="N27" s="5"/>
+      <c r="O27" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P27" s="7"/>
-    </row>
-    <row r="28" spans="1:16">
+      <c r="Q27">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2023,19 +2418,25 @@
       <c r="F28">
         <v>1103</v>
       </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
       <c r="L28">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="M28" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="N28" s="5"/>
       <c r="O28" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="P28" s="7"/>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="P28" s="8"/>
+      <c r="Q28">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2052,19 +2453,30 @@
       <c r="F29">
         <v>1083</v>
       </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
       <c r="L29">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="M29" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="N29" s="5"/>
       <c r="O29" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="P29" s="7"/>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="P29" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q29">
+        <v>1225</v>
+      </c>
+      <c r="R29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2081,19 +2493,30 @@
       <c r="F30">
         <v>998</v>
       </c>
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
       <c r="L30">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="M30" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="N30" s="5"/>
       <c r="O30" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="P30" s="7"/>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="P30" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q30">
+        <v>1296</v>
+      </c>
+      <c r="R30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2110,19 +2533,25 @@
       <c r="F31">
         <v>960</v>
       </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
       <c r="L31">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="M31" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="N31" s="5"/>
       <c r="O31" s="7" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="P31" s="7"/>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="Q31">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2139,19 +2568,30 @@
       <c r="F32">
         <v>927</v>
       </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
       <c r="L32">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="M32" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="N32" s="5"/>
       <c r="O32" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P32" s="8"/>
-    </row>
-    <row r="33" spans="1:16">
+      <c r="P32" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q32">
+        <v>5337</v>
+      </c>
+      <c r="R32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2168,17 +2608,25 @@
       <c r="F33">
         <v>885</v>
       </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
       <c r="L33">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="M33" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="N33" s="5"/>
-      <c r="O33" s="7"/>
+      <c r="O33" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P33" s="7"/>
-    </row>
-    <row r="34" spans="1:16">
+      <c r="Q33">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2195,6 +2643,9 @@
       <c r="F34">
         <v>885</v>
       </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
       <c r="L34">
         <v>32</v>
       </c>
@@ -2202,10 +2653,15 @@
         <v>69</v>
       </c>
       <c r="N34" s="5"/>
-      <c r="O34" s="7"/>
+      <c r="O34" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P34" s="7"/>
-    </row>
-    <row r="35" spans="1:16">
+      <c r="Q34">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2222,17 +2678,25 @@
       <c r="F35">
         <v>873</v>
       </c>
+      <c r="G35" t="b">
+        <v>0</v>
+      </c>
       <c r="L35">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="M35" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="N35" s="5"/>
-      <c r="O35" s="7"/>
+      <c r="O35" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P35" s="7"/>
-    </row>
-    <row r="36" spans="1:16">
+      <c r="Q35">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2249,17 +2713,25 @@
       <c r="F36">
         <v>825</v>
       </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
       <c r="L36">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="M36" t="s">
-        <v>71</v>
-      </c>
-      <c r="N36" s="6"/>
-      <c r="O36" s="7"/>
-      <c r="P36" s="7"/>
-    </row>
-    <row r="37" spans="1:16">
+        <v>86</v>
+      </c>
+      <c r="N36" s="5"/>
+      <c r="O36" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="P36" s="8"/>
+      <c r="Q36">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2276,17 +2748,30 @@
       <c r="F37">
         <v>824</v>
       </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
       <c r="L37">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="M37" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="N37" s="5"/>
-      <c r="O37" s="7"/>
-      <c r="P37" s="7"/>
-    </row>
-    <row r="38" spans="1:16">
+      <c r="O37" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P37" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q37">
+        <v>1083</v>
+      </c>
+      <c r="R37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2303,17 +2788,25 @@
       <c r="F38">
         <v>823</v>
       </c>
+      <c r="G38" t="b">
+        <v>0</v>
+      </c>
       <c r="L38">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M38" t="s">
-        <v>73</v>
-      </c>
-      <c r="N38" s="5"/>
-      <c r="O38" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="N38" s="6"/>
+      <c r="O38" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P38" s="7"/>
-    </row>
-    <row r="39" spans="1:16">
+      <c r="Q38">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2330,17 +2823,25 @@
       <c r="F39">
         <v>787</v>
       </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
       <c r="L39">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="M39" t="s">
-        <v>74</v>
-      </c>
-      <c r="N39" s="6"/>
-      <c r="O39" s="7"/>
-      <c r="P39" s="7"/>
-    </row>
-    <row r="40" spans="1:16">
+        <v>81</v>
+      </c>
+      <c r="N39" s="5"/>
+      <c r="O39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P39" s="8"/>
+      <c r="Q39">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2357,17 +2858,30 @@
       <c r="F40">
         <v>751</v>
       </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
       <c r="L40">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="M40" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="N40" s="5"/>
-      <c r="O40" s="7"/>
-      <c r="P40" s="7"/>
-    </row>
-    <row r="41" spans="1:16">
+      <c r="O40" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="P40" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q40">
+        <v>927</v>
+      </c>
+      <c r="R40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2384,17 +2898,25 @@
       <c r="F41">
         <v>718</v>
       </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
       <c r="L41">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="M41" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="N41" s="5"/>
-      <c r="O41" s="7"/>
+      <c r="O41" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P41" s="7"/>
-    </row>
-    <row r="42" spans="1:16">
+      <c r="Q41">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2402,24 +2924,34 @@
         <v>77</v>
       </c>
       <c r="C42" s="5"/>
-      <c r="D42" s="17"/>
+      <c r="D42" s="17" t="s">
+        <v>11</v>
+      </c>
       <c r="E42" s="17" t="s">
         <v>11</v>
       </c>
       <c r="F42">
         <v>718</v>
       </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
       <c r="L42">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="M42" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="N42" s="5"/>
-      <c r="O42" s="7"/>
+      <c r="O42" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P42" s="7"/>
-    </row>
-    <row r="43" spans="1:16">
+      <c r="Q42">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2436,17 +2968,30 @@
       <c r="F43">
         <v>709</v>
       </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
       <c r="L43">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="M43" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="N43" s="5"/>
-      <c r="O43" s="7"/>
-      <c r="P43" s="7"/>
-    </row>
-    <row r="44" spans="1:16">
+      <c r="O43" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P43" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q43">
+        <v>998</v>
+      </c>
+      <c r="R43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2463,17 +3008,30 @@
       <c r="F44">
         <v>707</v>
       </c>
+      <c r="G44" t="b">
+        <v>0</v>
+      </c>
       <c r="L44">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="M44" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="N44" s="5"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="8"/>
-    </row>
-    <row r="45" spans="1:16">
+      <c r="O44" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="P44" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q44">
+        <v>1876</v>
+      </c>
+      <c r="R44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2490,17 +3048,25 @@
       <c r="F45">
         <v>683</v>
       </c>
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
       <c r="L45">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="M45" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="N45" s="5"/>
-      <c r="O45" s="7"/>
-      <c r="P45" s="7"/>
-    </row>
-    <row r="46" spans="1:16">
+      <c r="O45" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="P45" s="8"/>
+      <c r="Q45">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2517,17 +3083,30 @@
       <c r="F46">
         <v>667</v>
       </c>
+      <c r="G46" t="b">
+        <v>1</v>
+      </c>
       <c r="L46">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="M46" t="s">
-        <v>81</v>
+        <v>46</v>
       </c>
       <c r="N46" s="5"/>
-      <c r="O46" s="8"/>
-      <c r="P46" s="8"/>
-    </row>
-    <row r="47" spans="1:16">
+      <c r="O46" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P46" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q46">
+        <v>4344</v>
+      </c>
+      <c r="R46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2544,17 +3123,32 @@
       <c r="F47">
         <v>661</v>
       </c>
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
       <c r="L47">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="M47" t="s">
-        <v>82</v>
-      </c>
-      <c r="N47" s="5"/>
-      <c r="O47" s="7"/>
-      <c r="P47" s="7"/>
-    </row>
-    <row r="48" spans="1:16">
+        <v>62</v>
+      </c>
+      <c r="N47" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="O47" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P47" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q47">
+        <v>1115</v>
+      </c>
+      <c r="R47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2571,15 +3165,23 @@
       <c r="F48">
         <v>649</v>
       </c>
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
       <c r="L48">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="M48" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="N48" s="5"/>
-      <c r="O48" s="7"/>
+      <c r="O48" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P48" s="7"/>
+      <c r="Q48">
+        <v>873</v>
+      </c>
     </row>
     <row r="49" spans="1:20">
       <c r="A49">
@@ -2598,15 +3200,23 @@
       <c r="F49">
         <v>641</v>
       </c>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
       <c r="L49">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="M49" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="N49" s="5"/>
-      <c r="O49" s="7"/>
+      <c r="O49" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P49" s="7"/>
+      <c r="Q49">
+        <v>718</v>
+      </c>
     </row>
     <row r="50" spans="1:20">
       <c r="A50">
@@ -2625,15 +3235,28 @@
       <c r="F50">
         <v>627</v>
       </c>
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
       <c r="L50">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="M50" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="N50" s="5"/>
-      <c r="O50" s="7"/>
-      <c r="P50" s="7"/>
+      <c r="O50" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P50" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q50">
+        <v>1812</v>
+      </c>
+      <c r="R50" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:20">
       <c r="A51">
@@ -2652,15 +3275,23 @@
       <c r="F51">
         <v>581</v>
       </c>
+      <c r="G51" t="b">
+        <v>1</v>
+      </c>
       <c r="L51">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="M51" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="N51" s="5"/>
-      <c r="O51" s="8"/>
+      <c r="O51" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="P51" s="8"/>
+      <c r="Q51">
+        <v>307</v>
+      </c>
     </row>
     <row r="52" spans="1:20">
       <c r="A52">
@@ -2679,15 +3310,23 @@
       <c r="F52">
         <v>495</v>
       </c>
+      <c r="G52" t="b">
+        <v>1</v>
+      </c>
       <c r="L52">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="M52" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="N52" s="5"/>
-      <c r="O52" s="7"/>
+      <c r="O52" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P52" s="7"/>
+      <c r="Q52">
+        <v>824</v>
+      </c>
     </row>
     <row r="53" spans="1:20">
       <c r="A53">
@@ -2704,15 +3343,23 @@
       <c r="F53">
         <v>323</v>
       </c>
+      <c r="G53" t="b">
+        <v>1</v>
+      </c>
       <c r="L53">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="M53" t="s">
-        <v>88</v>
-      </c>
-      <c r="N53" s="5"/>
-      <c r="O53" s="7"/>
+        <v>71</v>
+      </c>
+      <c r="N53" s="6"/>
+      <c r="O53" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="P53" s="7"/>
+      <c r="Q53">
+        <v>825</v>
+      </c>
     </row>
     <row r="54" spans="1:20">
       <c r="A54">
@@ -2731,15 +3378,28 @@
       <c r="F54">
         <v>313</v>
       </c>
+      <c r="G54" t="b">
+        <v>1</v>
+      </c>
       <c r="L54">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="M54" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="N54" s="5"/>
-      <c r="O54" s="7"/>
-      <c r="P54" s="7"/>
+      <c r="O54" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P54" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q54">
+        <v>2662</v>
+      </c>
+      <c r="R54" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="1:20">
       <c r="A55">
@@ -2758,15 +3418,28 @@
       <c r="F55">
         <v>307</v>
       </c>
+      <c r="G55" t="b">
+        <v>1</v>
+      </c>
       <c r="L55">
+        <v>16</v>
+      </c>
+      <c r="M55" t="s">
         <v>53</v>
       </c>
-      <c r="M55" t="s">
-        <v>89</v>
-      </c>
       <c r="N55" s="5"/>
-      <c r="O55" s="8"/>
-      <c r="P55" s="8"/>
+      <c r="O55" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P55" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q55">
+        <v>1802</v>
+      </c>
+      <c r="R55" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="1:20">
       <c r="A56">
@@ -2782,15 +3455,31 @@
       <c r="E56" s="17" t="s">
         <v>11</v>
       </c>
+      <c r="F56">
+        <v>1763</v>
+      </c>
+      <c r="G56" t="b">
+        <v>1</v>
+      </c>
       <c r="L56">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="M56" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="N56" s="5"/>
-      <c r="O56" s="8"/>
-      <c r="P56" s="8"/>
+      <c r="O56" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P56" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q56">
+        <v>3163</v>
+      </c>
+      <c r="R56" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="57" spans="1:20">
       <c r="A57">
@@ -2806,15 +3495,26 @@
       <c r="E57" s="17" t="s">
         <v>11</v>
       </c>
+      <c r="F57">
+        <v>3067</v>
+      </c>
+      <c r="G57" t="b">
+        <v>1</v>
+      </c>
       <c r="L57">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="M57" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="N57" s="5"/>
-      <c r="O57" s="8"/>
-      <c r="P57" s="8"/>
+      <c r="O57" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P57" s="7"/>
+      <c r="Q57">
+        <v>751</v>
+      </c>
     </row>
     <row r="58" spans="1:20">
       <c r="B58" s="5"/>
@@ -3460,7 +4160,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:F57">
+  <sortState ref="A3:J57">
     <sortCondition ref="A3:A57"/>
   </sortState>
   <mergeCells count="1">

</xml_diff>